<commit_message>
setting up excel input
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -14,9 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
-  <si>
-    <t>x</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>1:4:45</t>
+  </si>
+  <si>
+    <t>1|4|45</t>
+  </si>
+  <si>
+    <t>1 4 45</t>
+  </si>
+  <si>
+    <t>1-4-45</t>
   </si>
 </sst>
 </file>
@@ -376,98 +403,118 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="3.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="3.5764285714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="4.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="8.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="39">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="41.25">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="44.25">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="44.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generating experiment plan from excel spreadsheet
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -34,16 +34,10 @@
     <t>F</t>
   </si>
   <si>
-    <t>1:4:45</t>
-  </si>
-  <si>
-    <t>1|4|45</t>
+    <t>0 0 0</t>
   </si>
   <si>
     <t>1 4 45</t>
-  </si>
-  <si>
-    <t>1-4-45</t>
   </si>
 </sst>
 </file>
@@ -95,10 +89,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -437,84 +431,84 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="39">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="41.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="44.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="44.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>